<commit_message>
ssis form generator and loader
</commit_message>
<xml_diff>
--- a/Forms/Cash Monthly PDM form VER15 300512.xlsx
+++ b/Forms/Cash Monthly PDM form VER15 300512.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="28800" windowHeight="11175"/>
+    <workbookView xWindow="0" yWindow="6000" windowWidth="28800" windowHeight="11175"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,59 +24,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Code</t>
   </si>
   <si>
-    <t>CASH MONTHLY POST DISTRIBUTION MONITORING FORM PHASE 2- VER15 300512</t>
+    <t>Question</t>
   </si>
   <si>
-    <t>A: Personal Information</t>
+    <t>Answer</t>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>ID Number</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>District</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>Village</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>Registration Type</t>
-  </si>
-  <si>
-    <t>Codes for A4: 1 = Old registration from Phase I, 2 = New registration for phase II</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>Village Type</t>
-  </si>
-  <si>
-    <t>Codes for A5: 1 = Urban, 2 = Rural</t>
+    <t>FormHeading</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -104,8 +79,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,85 +362,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="73.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row spans="1:3" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>CASH MONTHLY POST DISTRIBUTION MONITORING FORM PHASE 2- VER15 300512</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>14</v>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>A: Personal Information</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>ID Number</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Village</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>Registration Type</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>Codes for A4: 1 = Old registration from Phase I, 2 = New registration for phase II</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>A5</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>Village Type</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>Codes for A5: 1 = Urban, 2 = Rural</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>A6</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>Are you short</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>TRUE/FALSE</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>